<commit_message>
update figures, create scripts per fig
</commit_message>
<xml_diff>
--- a/Data/Table1_functional_groups_dmb.xlsx
+++ b/Data/Table1_functional_groups_dmb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Barnas\Documents\Repositories\Community_Functional_Diversity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB69F235-801E-41A3-8CEB-3867F528043E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EB7ADF-4FD2-4610-8882-4CA00A001FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10572" yWindow="216" windowWidth="12336" windowHeight="14352" xr2:uid="{A94CFE18-78DA-43D0-9515-A795ED3F9922}"/>
+    <workbookView xWindow="9876" yWindow="120" windowWidth="12864" windowHeight="14604" xr2:uid="{A94CFE18-78DA-43D0-9515-A795ED3F9922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,56 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Morphology</t>
   </si>
   <si>
-    <t>Branched</t>
-  </si>
-  <si>
-    <t>Cushion-like</t>
-  </si>
-  <si>
-    <t>Digitate</t>
-  </si>
-  <si>
-    <t>Encrusting</t>
-  </si>
-  <si>
-    <t>Filamentous</t>
-  </si>
-  <si>
-    <t>Foliose</t>
-  </si>
-  <si>
-    <t>Massive</t>
-  </si>
-  <si>
-    <t>Mushroom</t>
-  </si>
-  <si>
-    <t>Polypoid</t>
-  </si>
-  <si>
-    <t>Spherical</t>
-  </si>
-  <si>
-    <t>Stolonial</t>
-  </si>
-  <si>
-    <t>Taxonomic Group</t>
-  </si>
-  <si>
-    <t>Anemone</t>
-  </si>
-  <si>
-    <t>Corallimorpharia</t>
-  </si>
-  <si>
-    <t>Scleractinia</t>
-  </si>
-  <si>
     <t>Chlorophyta</t>
   </si>
   <si>
@@ -95,27 +50,12 @@
     <t>Rhodophyta</t>
   </si>
   <si>
-    <t>Demospongiae</t>
-  </si>
-  <si>
     <t>Cyanobacteria</t>
   </si>
   <si>
     <t>Calcification</t>
   </si>
   <si>
-    <t>Non-calcified</t>
-  </si>
-  <si>
-    <t>Articulated calcification</t>
-  </si>
-  <si>
-    <t>Non-articulated calcification</t>
-  </si>
-  <si>
-    <t>Hermatypic</t>
-  </si>
-  <si>
     <t>Symbiosis</t>
   </si>
   <si>
@@ -195,6 +135,60 @@
   </si>
   <si>
     <t>Perennial</t>
+  </si>
+  <si>
+    <t>Cnidaria</t>
+  </si>
+  <si>
+    <t>Porifera</t>
+  </si>
+  <si>
+    <t>Branched (Br)</t>
+  </si>
+  <si>
+    <t>Cushion-like (Cushion)</t>
+  </si>
+  <si>
+    <t>Digitate (Dig)</t>
+  </si>
+  <si>
+    <t>Encrusting (Enc)</t>
+  </si>
+  <si>
+    <t>Filamentous (Fil)</t>
+  </si>
+  <si>
+    <t>Foliose (Fol)</t>
+  </si>
+  <si>
+    <t>Massive (Mas)</t>
+  </si>
+  <si>
+    <t>Mushroom (Mush)</t>
+  </si>
+  <si>
+    <t>Polypoid (Poly)</t>
+  </si>
+  <si>
+    <t>Spherical (Sph)</t>
+  </si>
+  <si>
+    <t>Stolonial (Stol)</t>
+  </si>
+  <si>
+    <t>Phyla</t>
+  </si>
+  <si>
+    <t>Non-calcified (NC)</t>
+  </si>
+  <si>
+    <t>Articulated (AC)</t>
+  </si>
+  <si>
+    <t>Non-articulated (Non-AC)</t>
+  </si>
+  <si>
+    <t>Hermatypic (Herm)</t>
   </si>
 </sst>
 </file>
@@ -549,7 +543,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,182 +553,176 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
         <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>